<commit_message>
Adding files for everyone
</commit_message>
<xml_diff>
--- a/customer1.xlsx
+++ b/customer1.xlsx
@@ -8,30 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samdsouza/Documents/EatUp/EatUp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59ADBAA0-B187-FD48-AE58-EECCF32BAF8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B653FDF-1811-7842-9759-FA70CB2F874F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="640" windowWidth="28040" windowHeight="17440" xr2:uid="{E358115F-6BB9-A043-B54C-E81150EFBE34}"/>
+    <workbookView xWindow="3260" yWindow="880" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">Customer ID </t>
   </si>
@@ -54,16 +43,64 @@
     <t xml:space="preserve">Rewards Earned </t>
   </si>
   <si>
+    <t xml:space="preserve">Rewards Claimed </t>
+  </si>
+  <si>
+    <t>3/19/2020'</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chick Fil A </t>
   </si>
   <si>
+    <t>3/20/2020'</t>
+  </si>
+  <si>
     <t xml:space="preserve">AeroTek </t>
   </si>
   <si>
-    <t>3/20/2020'</t>
-  </si>
-  <si>
-    <t>3/19/2020'</t>
+    <t>3/25/2020'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BlackBelly </t>
+  </si>
+  <si>
+    <t>3/26/2020'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Buff </t>
+  </si>
+  <si>
+    <t>3/29/2020'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oak </t>
+  </si>
+  <si>
+    <t>3/30/2020'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The West End Tavern </t>
+  </si>
+  <si>
+    <t>3/31/2020'</t>
+  </si>
+  <si>
+    <t>ChopHouse</t>
+  </si>
+  <si>
+    <t>4/1/2020'</t>
+  </si>
+  <si>
+    <t>Via Perla</t>
+  </si>
+  <si>
+    <t>4/2/2020'</t>
+  </si>
+  <si>
+    <t>Pizzeria Locale</t>
+  </si>
+  <si>
+    <t>55.76</t>
   </si>
 </sst>
 </file>
@@ -99,9 +136,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,21 +453,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8326E8F2-4272-3E4F-B544-D23441530480}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,7 +477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -445,7 +485,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -458,13 +498,16 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>12.99</v>
@@ -473,18 +516,116 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>7.55</v>
       </c>
       <c r="D6">
         <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>109.55</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>35.99</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>75.760000000000005</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>25.26</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>56.75</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12">
+        <v>60.74</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>